<commit_message>
rendering unique and import functionality completed
</commit_message>
<xml_diff>
--- a/backend/public/uploads/Book1.xlsx
+++ b/backend/public/uploads/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Phone</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>sdfdsf</t>
   </si>
   <si>
@@ -43,22 +40,16 @@
     <t>dfd</t>
   </si>
   <si>
+    <t>jkl</t>
+  </si>
+  <si>
+    <t>Yash</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
     <t>f</t>
-  </si>
-  <si>
-    <t>sdfsd</t>
-  </si>
-  <si>
-    <t>dfs</t>
-  </si>
-  <si>
-    <t>df</t>
-  </si>
-  <si>
-    <t>Yash</t>
-  </si>
-  <si>
-    <t>fd</t>
   </si>
 </sst>
 </file>
@@ -66,8 +57,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
@@ -80,6 +71,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -88,23 +101,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -113,21 +120,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -141,6 +133,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -165,16 +171,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -188,15 +202,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -204,21 +210,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -233,67 +224,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,115 +404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -429,11 +420,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -479,33 +483,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -524,20 +506,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -547,130 +538,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -997,13 +988,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -1022,35 +1013,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="3" ht="30" customHeight="1" spans="1:5">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3">
         <v>89</v>
@@ -1058,35 +1032,18 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>2543</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sending mail task completed
</commit_message>
<xml_diff>
--- a/backend/public/uploads/Book1.xlsx
+++ b/backend/public/uploads/Book1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -71,6 +71,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -78,16 +116,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -96,22 +127,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,6 +148,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -140,39 +170,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,29 +202,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -224,187 +224,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -422,22 +422,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -453,15 +438,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -483,11 +459,33 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -509,9 +507,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,148 +520,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -991,7 +991,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1013,6 +1013,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" ht="30" customHeight="1" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>89</v>
+      </c>
+    </row>
     <row r="3" ht="30" customHeight="1" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>

</xml_diff>